<commit_message>
Day 5 (Linked List End)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psharm03\DS-Algo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psharm03\Documents\GitHub\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6CF439-8797-48CC-93A4-EFC23DB1C3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9D6888-7FB8-45C8-93FF-E814847C6527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="475">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -519,12 +519,6 @@
     <t>Flatten a Linked List</t>
   </si>
   <si>
-    <t>Clone a linked list with next and random pointer</t>
-  </si>
-  <si>
-    <t>Merge K sorted Linked list</t>
-  </si>
-  <si>
     <t>Multiply 2 no. represented by LL</t>
   </si>
   <si>
@@ -1453,6 +1447,27 @@
   </si>
   <si>
     <t>Sort a LL of 0's, 1's and 2's (Replacing data and replacing links)</t>
+  </si>
+  <si>
+    <t>O(NKlogN)</t>
+  </si>
+  <si>
+    <t>Merge K sorted Linked list [Try Min-Heap later] (merge in 2-2 pairs using divide and conqure)</t>
+  </si>
+  <si>
+    <t>Space Complexity</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>Clone a linked list with next and random pointer [3 approaches]</t>
+  </si>
+  <si>
+    <t>O(nlogn)</t>
+  </si>
+  <si>
+    <t>O(nm)</t>
   </si>
 </sst>
 </file>
@@ -1628,8 +1643,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AD70A15-AEF6-44CD-8C33-15789C17FB29}" name="Table1" displayName="Table1" ref="H1:H3" totalsRowShown="0">
-  <autoFilter ref="H1:H3" xr:uid="{7AD70A15-AEF6-44CD-8C33-15789C17FB29}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7AD70A15-AEF6-44CD-8C33-15789C17FB29}" name="Table1" displayName="Table1" ref="I1:I3" totalsRowShown="0">
+  <autoFilter ref="I1:I3" xr:uid="{7AD70A15-AEF6-44CD-8C33-15789C17FB29}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{F4DB1A79-9427-4F35-84F9-E657ABB8DDC1}" name="Column1"/>
   </tableColumns>
@@ -1945,17 +1960,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="11" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -1968,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
-  <dimension ref="A1:H481"/>
+  <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="F166" sqref="F166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -1981,32 +1996,33 @@
     <col min="3" max="3" width="87.4140625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25">
+    <row r="1" spans="1:9" ht="25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="C2" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="I2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="I3" t="s">
         <v>458</v>
       </c>
-      <c r="H2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="H3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="21">
+    </row>
+    <row r="4" spans="1:9" ht="21">
       <c r="A4" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -2018,13 +2034,16 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>460</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="21">
+    <row r="6" spans="1:9" ht="21">
       <c r="A6" s="12">
         <v>1</v>
       </c>
@@ -2035,13 +2054,14 @@
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="21">
+        <v>461</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" ht="21">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -2052,13 +2072,14 @@
         <v>6</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="21">
+        <v>461</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="21">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2070,7 +2091,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="21">
+    <row r="9" spans="1:9" ht="21">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2082,7 +2103,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="21">
+    <row r="10" spans="1:9" ht="21">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2094,7 +2115,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="21">
+    <row r="11" spans="1:9" ht="21">
       <c r="A11">
         <v>6</v>
       </c>
@@ -2106,7 +2127,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="21">
+    <row r="12" spans="1:9" ht="21">
       <c r="A12">
         <v>7</v>
       </c>
@@ -2118,7 +2139,7 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="21">
+    <row r="13" spans="1:9" ht="21">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2130,7 +2151,7 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="21">
+    <row r="14" spans="1:9" ht="21">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2142,7 +2163,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="21">
+    <row r="15" spans="1:9" ht="21">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2154,7 +2175,7 @@
       </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="21">
+    <row r="16" spans="1:9" ht="21">
       <c r="A16">
         <v>11</v>
       </c>
@@ -3463,7 +3484,7 @@
       </c>
       <c r="D128" s="4"/>
     </row>
-    <row r="129" spans="1:6" ht="21">
+    <row r="129" spans="1:7" ht="21">
       <c r="A129">
         <v>118</v>
       </c>
@@ -3475,7 +3496,7 @@
       </c>
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="1:6" ht="21">
+    <row r="130" spans="1:7" ht="21">
       <c r="A130">
         <v>119</v>
       </c>
@@ -3487,7 +3508,7 @@
       </c>
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="1:6" ht="21">
+    <row r="131" spans="1:7" ht="21">
       <c r="A131">
         <v>120</v>
       </c>
@@ -3499,7 +3520,7 @@
       </c>
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="1:6" ht="21">
+    <row r="132" spans="1:7" ht="21">
       <c r="A132">
         <v>121</v>
       </c>
@@ -3511,7 +3532,7 @@
       </c>
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="1:6" ht="21">
+    <row r="133" spans="1:7" ht="21">
       <c r="A133">
         <v>122</v>
       </c>
@@ -3523,7 +3544,7 @@
       </c>
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="1:6" ht="21">
+    <row r="134" spans="1:7" ht="21">
       <c r="A134">
         <v>123</v>
       </c>
@@ -3535,7 +3556,7 @@
       </c>
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="1:6" ht="21">
+    <row r="135" spans="1:7" ht="21">
       <c r="A135">
         <v>124</v>
       </c>
@@ -3547,7 +3568,7 @@
       </c>
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="1:6" ht="21">
+    <row r="136" spans="1:7" ht="21">
       <c r="A136">
         <v>125</v>
       </c>
@@ -3559,14 +3580,14 @@
       </c>
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:7">
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="1:6" ht="21">
+    <row r="138" spans="1:7" ht="21">
       <c r="C138" s="7"/>
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="1:6" ht="21">
+    <row r="139" spans="1:7" ht="21">
       <c r="A139" s="12">
         <v>126</v>
       </c>
@@ -3577,16 +3598,17 @@
         <v>134</v>
       </c>
       <c r="D139" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E139" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F139">
+        <v>461</v>
+      </c>
+      <c r="F139" s="12"/>
+      <c r="G139">
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="21">
+    <row r="140" spans="1:7" ht="21">
       <c r="A140" s="12">
         <v>127</v>
       </c>
@@ -3597,16 +3619,17 @@
         <v>135</v>
       </c>
       <c r="D140" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E140" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F140">
+        <v>461</v>
+      </c>
+      <c r="F140" s="12"/>
+      <c r="G140">
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="21">
+    <row r="141" spans="1:7" ht="21">
       <c r="A141" s="12">
         <v>128</v>
       </c>
@@ -3617,16 +3640,17 @@
         <v>136</v>
       </c>
       <c r="D141" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E141" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F141">
+        <v>461</v>
+      </c>
+      <c r="F141" s="12"/>
+      <c r="G141">
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="21">
+    <row r="142" spans="1:7" ht="21">
       <c r="A142" s="12">
         <v>129</v>
       </c>
@@ -3634,19 +3658,20 @@
         <v>133</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D142" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E142" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F142">
+        <v>461</v>
+      </c>
+      <c r="F142" s="12"/>
+      <c r="G142">
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="21">
+    <row r="143" spans="1:7" ht="21">
       <c r="A143" s="12">
         <v>130</v>
       </c>
@@ -3657,16 +3682,17 @@
         <v>137</v>
       </c>
       <c r="D143" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E143" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F143">
+        <v>461</v>
+      </c>
+      <c r="F143" s="12"/>
+      <c r="G143">
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="21">
+    <row r="144" spans="1:7" ht="21">
       <c r="A144" s="12">
         <v>131</v>
       </c>
@@ -3674,17 +3700,18 @@
         <v>133</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D144" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E144" s="12"/>
-      <c r="F144">
+      <c r="F144" s="12"/>
+      <c r="G144">
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="21">
+    <row r="145" spans="1:7" ht="21">
       <c r="A145" s="12">
         <v>132</v>
       </c>
@@ -3692,17 +3719,18 @@
         <v>133</v>
       </c>
       <c r="C145" s="14" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D145" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E145" s="12"/>
-      <c r="F145">
+      <c r="F145" s="12"/>
+      <c r="G145">
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="21">
+    <row r="146" spans="1:7" ht="21">
       <c r="A146">
         <v>133</v>
       </c>
@@ -3713,11 +3741,11 @@
         <v>138</v>
       </c>
       <c r="D146" s="4"/>
-      <c r="F146">
+      <c r="G146">
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="21">
+    <row r="147" spans="1:7" ht="21">
       <c r="A147">
         <v>134</v>
       </c>
@@ -3728,11 +3756,11 @@
         <v>139</v>
       </c>
       <c r="D147" s="4"/>
-      <c r="F147">
+      <c r="G147">
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="21">
+    <row r="148" spans="1:7" ht="21">
       <c r="A148">
         <v>135</v>
       </c>
@@ -3743,11 +3771,11 @@
         <v>140</v>
       </c>
       <c r="D148" s="4"/>
-      <c r="F148">
+      <c r="G148">
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="21">
+    <row r="149" spans="1:7" ht="21">
       <c r="A149">
         <v>136</v>
       </c>
@@ -3758,11 +3786,11 @@
         <v>141</v>
       </c>
       <c r="D149" s="4"/>
-      <c r="F149">
+      <c r="G149">
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="21">
+    <row r="150" spans="1:7" ht="21">
       <c r="A150">
         <v>137</v>
       </c>
@@ -3773,26 +3801,34 @@
         <v>142</v>
       </c>
       <c r="D150" s="4"/>
-      <c r="F150">
+      <c r="G150">
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="21">
-      <c r="A151">
+    <row r="151" spans="1:7" ht="21">
+      <c r="A151" s="12">
         <v>138</v>
       </c>
-      <c r="B151" s="8" t="s">
+      <c r="B151" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C151" s="6" t="s">
+      <c r="C151" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D151" s="4"/>
-      <c r="F151">
+      <c r="D151" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E151" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="F151" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="G151">
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="21">
+    <row r="152" spans="1:7" ht="21">
       <c r="A152">
         <v>139</v>
       </c>
@@ -3803,11 +3839,11 @@
         <v>144</v>
       </c>
       <c r="D152" s="4"/>
-      <c r="F152">
+      <c r="G152">
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="21">
+    <row r="153" spans="1:7" ht="21">
       <c r="A153" s="12">
         <v>140</v>
       </c>
@@ -3815,19 +3851,20 @@
         <v>133</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D153" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E153" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F153">
+        <v>461</v>
+      </c>
+      <c r="F153" s="12"/>
+      <c r="G153">
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="21">
+    <row r="154" spans="1:7" ht="21">
       <c r="A154" s="12">
         <v>141</v>
       </c>
@@ -3838,16 +3875,17 @@
         <v>145</v>
       </c>
       <c r="D154" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E154" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F154">
+        <v>461</v>
+      </c>
+      <c r="F154" s="12"/>
+      <c r="G154">
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="21">
+    <row r="155" spans="1:7" ht="21">
       <c r="A155">
         <v>142</v>
       </c>
@@ -3858,26 +3896,30 @@
         <v>146</v>
       </c>
       <c r="D155" s="4"/>
-      <c r="F155">
+      <c r="G155">
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="21">
-      <c r="A156">
+    <row r="156" spans="1:7" ht="21">
+      <c r="A156" s="12">
         <v>143</v>
       </c>
-      <c r="B156" s="8" t="s">
+      <c r="B156" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C156" s="6" t="s">
+      <c r="C156" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="D156" s="4"/>
-      <c r="F156">
+      <c r="D156" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E156" s="12"/>
+      <c r="F156" s="12"/>
+      <c r="G156">
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="21">
+    <row r="157" spans="1:7" ht="21">
       <c r="A157">
         <v>144</v>
       </c>
@@ -3888,11 +3930,11 @@
         <v>148</v>
       </c>
       <c r="D157" s="4"/>
-      <c r="F157">
+      <c r="G157">
         <v>19</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="21">
+    <row r="158" spans="1:7" ht="21">
       <c r="A158">
         <v>145</v>
       </c>
@@ -3903,11 +3945,11 @@
         <v>149</v>
       </c>
       <c r="D158" s="4"/>
-      <c r="F158">
+      <c r="G158">
         <v>20</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="21">
+    <row r="159" spans="1:7" ht="21">
       <c r="A159">
         <v>146</v>
       </c>
@@ -3918,11 +3960,11 @@
         <v>150</v>
       </c>
       <c r="D159" s="4"/>
-      <c r="F159">
+      <c r="G159">
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="21">
+    <row r="160" spans="1:7" ht="21">
       <c r="A160">
         <v>147</v>
       </c>
@@ -3933,11 +3975,11 @@
         <v>151</v>
       </c>
       <c r="D160" s="4"/>
-      <c r="F160">
+      <c r="G160">
         <v>22</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="21">
+    <row r="161" spans="1:7" ht="21">
       <c r="A161">
         <v>148</v>
       </c>
@@ -3948,11 +3990,11 @@
         <v>152</v>
       </c>
       <c r="D161" s="4"/>
-      <c r="F161">
+      <c r="G161">
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="21">
+    <row r="162" spans="1:7" ht="21">
       <c r="A162">
         <v>149</v>
       </c>
@@ -3963,11 +4005,11 @@
         <v>153</v>
       </c>
       <c r="D162" s="4"/>
-      <c r="F162">
+      <c r="G162">
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="21">
+    <row r="163" spans="1:7" ht="21">
       <c r="A163">
         <v>150</v>
       </c>
@@ -3978,11 +4020,11 @@
         <v>154</v>
       </c>
       <c r="D163" s="4"/>
-      <c r="F163">
+      <c r="G163">
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="21">
+    <row r="164" spans="1:7" ht="21">
       <c r="A164">
         <v>151</v>
       </c>
@@ -3993,11 +4035,11 @@
         <v>155</v>
       </c>
       <c r="D164" s="4"/>
-      <c r="F164">
+      <c r="G164">
         <v>26</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="21">
+    <row r="165" spans="1:7" ht="21">
       <c r="A165">
         <v>152</v>
       </c>
@@ -4008,26 +4050,34 @@
         <v>156</v>
       </c>
       <c r="D165" s="4"/>
-      <c r="F165">
+      <c r="G165">
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="21">
-      <c r="A166">
+    <row r="166" spans="1:7" ht="21">
+      <c r="A166" s="12">
         <v>153</v>
       </c>
-      <c r="B166" s="8" t="s">
+      <c r="B166" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C166" s="6" t="s">
+      <c r="C166" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="D166" s="4"/>
-      <c r="F166">
+      <c r="D166" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E166" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="F166" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="G166">
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="21">
+    <row r="167" spans="1:7" ht="21">
       <c r="A167" s="12">
         <v>154</v>
       </c>
@@ -4035,49 +4085,64 @@
         <v>133</v>
       </c>
       <c r="C167" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="D167" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E167" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="F167" s="12"/>
+      <c r="G167">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="21">
+      <c r="A168" s="12">
+        <v>155</v>
+      </c>
+      <c r="B168" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C168" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="D168" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E168" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="F168" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="G168">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="21">
+      <c r="A169" s="12">
+        <v>156</v>
+      </c>
+      <c r="B169" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C169" s="14" t="s">
         <v>469</v>
       </c>
-      <c r="D167" s="15" t="s">
-        <v>459</v>
-      </c>
-      <c r="E167" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="F167">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="21">
-      <c r="A168">
-        <v>155</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C168" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D168" s="4"/>
-      <c r="F168">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="21">
-      <c r="A169">
-        <v>156</v>
-      </c>
-      <c r="B169" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C169" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D169" s="4"/>
-      <c r="F169">
+      <c r="D169" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="E169" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="F169" s="12"/>
+      <c r="G169">
         <v>31</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="21">
+    <row r="170" spans="1:7" ht="21">
       <c r="A170">
         <v>157</v>
       </c>
@@ -4085,14 +4150,14 @@
         <v>133</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D170" s="4"/>
-      <c r="F170">
+      <c r="G170">
         <v>32</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="21">
+    <row r="171" spans="1:7" ht="21">
       <c r="A171">
         <v>158</v>
       </c>
@@ -4100,14 +4165,14 @@
         <v>133</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D171" s="4"/>
-      <c r="F171">
+      <c r="G171">
         <v>33</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="21">
+    <row r="172" spans="1:7" ht="21">
       <c r="A172">
         <v>159</v>
       </c>
@@ -4115,14 +4180,14 @@
         <v>133</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D172" s="4"/>
-      <c r="F172">
+      <c r="G172">
         <v>34</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="21">
+    <row r="173" spans="1:7" ht="21">
       <c r="A173">
         <v>160</v>
       </c>
@@ -4130,14 +4195,14 @@
         <v>133</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D173" s="4"/>
-      <c r="F173">
+      <c r="G173">
         <v>35</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="21">
+    <row r="174" spans="1:7" ht="21">
       <c r="A174">
         <v>161</v>
       </c>
@@ -4145,17 +4210,17 @@
         <v>133</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D174" s="4"/>
-      <c r="F174">
+      <c r="G174">
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:7">
       <c r="D175" s="4"/>
     </row>
-    <row r="176" spans="1:6" ht="21">
+    <row r="176" spans="1:7" ht="21">
       <c r="C176" s="7"/>
       <c r="D176" s="4"/>
     </row>
@@ -4164,10 +4229,10 @@
         <v>162</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D177" s="4"/>
     </row>
@@ -4176,10 +4241,10 @@
         <v>163</v>
       </c>
       <c r="B178" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C178" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="C178" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="D178" s="4"/>
     </row>
@@ -4188,10 +4253,10 @@
         <v>164</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D179" s="4"/>
     </row>
@@ -4200,10 +4265,10 @@
         <v>165</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D180" s="4"/>
     </row>
@@ -4212,10 +4277,10 @@
         <v>166</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D181" s="4"/>
     </row>
@@ -4224,10 +4289,10 @@
         <v>167</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D182" s="4"/>
     </row>
@@ -4236,10 +4301,10 @@
         <v>168</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D183" s="4"/>
     </row>
@@ -4248,10 +4313,10 @@
         <v>169</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D184" s="4"/>
     </row>
@@ -4260,10 +4325,10 @@
         <v>170</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D185" s="4"/>
     </row>
@@ -4272,10 +4337,10 @@
         <v>171</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D186" s="4"/>
     </row>
@@ -4284,10 +4349,10 @@
         <v>172</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D187" s="4"/>
     </row>
@@ -4296,10 +4361,10 @@
         <v>173</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D188" s="4"/>
     </row>
@@ -4308,10 +4373,10 @@
         <v>174</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D189" s="4"/>
     </row>
@@ -4320,10 +4385,10 @@
         <v>175</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D190" s="4"/>
     </row>
@@ -4332,10 +4397,10 @@
         <v>176</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C191" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D191" s="4"/>
     </row>
@@ -4344,10 +4409,10 @@
         <v>177</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D192" s="4"/>
     </row>
@@ -4356,10 +4421,10 @@
         <v>178</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C193" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D193" s="4"/>
     </row>
@@ -4368,10 +4433,10 @@
         <v>179</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D194" s="4"/>
     </row>
@@ -4380,10 +4445,10 @@
         <v>180</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D195" s="4"/>
     </row>
@@ -4392,10 +4457,10 @@
         <v>181</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D196" s="4"/>
     </row>
@@ -4404,10 +4469,10 @@
         <v>182</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D197" s="4"/>
     </row>
@@ -4416,10 +4481,10 @@
         <v>183</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C198" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D198" s="4"/>
     </row>
@@ -4428,10 +4493,10 @@
         <v>184</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D199" s="4"/>
     </row>
@@ -4440,10 +4505,10 @@
         <v>185</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D200" s="4"/>
     </row>
@@ -4452,10 +4517,10 @@
         <v>186</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C201" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D201" s="4"/>
     </row>
@@ -4464,10 +4529,10 @@
         <v>187</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C202" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D202" s="4"/>
     </row>
@@ -4476,10 +4541,10 @@
         <v>188</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C203" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D203" s="4"/>
     </row>
@@ -4488,10 +4553,10 @@
         <v>189</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D204" s="4"/>
     </row>
@@ -4500,10 +4565,10 @@
         <v>190</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D205" s="4"/>
     </row>
@@ -4512,10 +4577,10 @@
         <v>191</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D206" s="4"/>
     </row>
@@ -4524,10 +4589,10 @@
         <v>192</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C207" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D207" s="4"/>
     </row>
@@ -4536,10 +4601,10 @@
         <v>193</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C208" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D208" s="4"/>
     </row>
@@ -4548,10 +4613,10 @@
         <v>194</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C209" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D209" s="4"/>
     </row>
@@ -4560,10 +4625,10 @@
         <v>195</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C210" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D210" s="4"/>
     </row>
@@ -4572,10 +4637,10 @@
         <v>196</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C211" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D211" s="4"/>
     </row>
@@ -4594,10 +4659,10 @@
         <v>197</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C214" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D214" s="4"/>
     </row>
@@ -4606,10 +4671,10 @@
         <v>198</v>
       </c>
       <c r="B215" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C215" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="C215" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="D215" s="4"/>
     </row>
@@ -4618,10 +4683,10 @@
         <v>199</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C216" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D216" s="4"/>
     </row>
@@ -4630,10 +4695,10 @@
         <v>200</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D217" s="4"/>
     </row>
@@ -4642,10 +4707,10 @@
         <v>201</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C218" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D218" s="4"/>
     </row>
@@ -4654,10 +4719,10 @@
         <v>202</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D219" s="4"/>
     </row>
@@ -4666,10 +4731,10 @@
         <v>203</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D220" s="4"/>
     </row>
@@ -4678,10 +4743,10 @@
         <v>204</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D221" s="4"/>
     </row>
@@ -4690,10 +4755,10 @@
         <v>205</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C222" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D222" s="4"/>
     </row>
@@ -4702,10 +4767,10 @@
         <v>206</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C223" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D223" s="4"/>
     </row>
@@ -4714,10 +4779,10 @@
         <v>207</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C224" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D224" s="4"/>
     </row>
@@ -4726,10 +4791,10 @@
         <v>208</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C225" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D225" s="4"/>
     </row>
@@ -4738,10 +4803,10 @@
         <v>209</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D226" s="4"/>
     </row>
@@ -4750,10 +4815,10 @@
         <v>210</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D227" s="4"/>
     </row>
@@ -4762,10 +4827,10 @@
         <v>211</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C228" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D228" s="4"/>
     </row>
@@ -4774,10 +4839,10 @@
         <v>212</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D229" s="4"/>
     </row>
@@ -4786,10 +4851,10 @@
         <v>213</v>
       </c>
       <c r="B230" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D230" s="4"/>
     </row>
@@ -4798,10 +4863,10 @@
         <v>214</v>
       </c>
       <c r="B231" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C231" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D231" s="4"/>
     </row>
@@ -4810,10 +4875,10 @@
         <v>215</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D232" s="4"/>
     </row>
@@ -4822,10 +4887,10 @@
         <v>216</v>
       </c>
       <c r="B233" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C233" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D233" s="4"/>
     </row>
@@ -4834,10 +4899,10 @@
         <v>217</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C234" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D234" s="4"/>
     </row>
@@ -4846,10 +4911,10 @@
         <v>218</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C235" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D235" s="4"/>
     </row>
@@ -4866,10 +4931,10 @@
         <v>219</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C238" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D238" s="4"/>
     </row>
@@ -4878,10 +4943,10 @@
         <v>220</v>
       </c>
       <c r="B239" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C239" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="C239" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="D239" s="4"/>
     </row>
@@ -4890,10 +4955,10 @@
         <v>221</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C240" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D240" s="4"/>
     </row>
@@ -4902,10 +4967,10 @@
         <v>222</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C241" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D241" s="4"/>
     </row>
@@ -4914,10 +4979,10 @@
         <v>223</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C242" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D242" s="4"/>
     </row>
@@ -4926,10 +4991,10 @@
         <v>224</v>
       </c>
       <c r="B243" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C243" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D243" s="4"/>
     </row>
@@ -4938,10 +5003,10 @@
         <v>225</v>
       </c>
       <c r="B244" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C244" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D244" s="4"/>
     </row>
@@ -4950,10 +5015,10 @@
         <v>226</v>
       </c>
       <c r="B245" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D245" s="4"/>
     </row>
@@ -4962,10 +5027,10 @@
         <v>227</v>
       </c>
       <c r="B246" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C246" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D246" s="4"/>
     </row>
@@ -4974,10 +5039,10 @@
         <v>228</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C247" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D247" s="4"/>
     </row>
@@ -4986,10 +5051,10 @@
         <v>229</v>
       </c>
       <c r="B248" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C248" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D248" s="4"/>
     </row>
@@ -4998,10 +5063,10 @@
         <v>230</v>
       </c>
       <c r="B249" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C249" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D249" s="4"/>
     </row>
@@ -5010,10 +5075,10 @@
         <v>231</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C250" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D250" s="4"/>
     </row>
@@ -5022,10 +5087,10 @@
         <v>232</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C251" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D251" s="4"/>
     </row>
@@ -5034,10 +5099,10 @@
         <v>233</v>
       </c>
       <c r="B252" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C252" s="6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D252" s="4"/>
     </row>
@@ -5046,10 +5111,10 @@
         <v>234</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C253" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D253" s="4"/>
     </row>
@@ -5058,10 +5123,10 @@
         <v>235</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C254" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D254" s="4"/>
     </row>
@@ -5070,10 +5135,10 @@
         <v>236</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C255" s="6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D255" s="4"/>
     </row>
@@ -5082,10 +5147,10 @@
         <v>237</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C256" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D256" s="4"/>
     </row>
@@ -5094,10 +5159,10 @@
         <v>238</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C257" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D257" s="4"/>
     </row>
@@ -5106,10 +5171,10 @@
         <v>239</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C258" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D258" s="4"/>
     </row>
@@ -5118,10 +5183,10 @@
         <v>240</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C259" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D259" s="4"/>
     </row>
@@ -5130,10 +5195,10 @@
         <v>241</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C260" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D260" s="4"/>
     </row>
@@ -5142,10 +5207,10 @@
         <v>242</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C261" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D261" s="4"/>
     </row>
@@ -5154,10 +5219,10 @@
         <v>243</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C262" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D262" s="4"/>
     </row>
@@ -5166,10 +5231,10 @@
         <v>244</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C263" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D263" s="4"/>
     </row>
@@ -5178,10 +5243,10 @@
         <v>245</v>
       </c>
       <c r="B264" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C264" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D264" s="4"/>
     </row>
@@ -5190,10 +5255,10 @@
         <v>246</v>
       </c>
       <c r="B265" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C265" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D265" s="4"/>
     </row>
@@ -5202,10 +5267,10 @@
         <v>247</v>
       </c>
       <c r="B266" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C266" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D266" s="4"/>
     </row>
@@ -5214,10 +5279,10 @@
         <v>248</v>
       </c>
       <c r="B267" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C267" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D267" s="4"/>
     </row>
@@ -5226,10 +5291,10 @@
         <v>249</v>
       </c>
       <c r="B268" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C268" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D268" s="4"/>
     </row>
@@ -5238,10 +5303,10 @@
         <v>250</v>
       </c>
       <c r="B269" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C269" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D269" s="4"/>
     </row>
@@ -5250,10 +5315,10 @@
         <v>251</v>
       </c>
       <c r="B270" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C270" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D270" s="4"/>
     </row>
@@ -5262,7 +5327,7 @@
         <v>252</v>
       </c>
       <c r="B271" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C271" s="6" t="s">
         <v>86</v>
@@ -5274,10 +5339,10 @@
         <v>253</v>
       </c>
       <c r="B272" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C272" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D272" s="4"/>
     </row>
@@ -5294,10 +5359,10 @@
         <v>254</v>
       </c>
       <c r="B275" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C275" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D275" s="4"/>
     </row>
@@ -5306,10 +5371,10 @@
         <v>255</v>
       </c>
       <c r="B276" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C276" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="C276" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="D276" s="4"/>
     </row>
@@ -5318,10 +5383,10 @@
         <v>256</v>
       </c>
       <c r="B277" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C277" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D277" s="4"/>
     </row>
@@ -5330,10 +5395,10 @@
         <v>257</v>
       </c>
       <c r="B278" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C278" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D278" s="4"/>
     </row>
@@ -5342,10 +5407,10 @@
         <v>258</v>
       </c>
       <c r="B279" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C279" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D279" s="4"/>
     </row>
@@ -5354,10 +5419,10 @@
         <v>259</v>
       </c>
       <c r="B280" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C280" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D280" s="4"/>
     </row>
@@ -5366,10 +5431,10 @@
         <v>260</v>
       </c>
       <c r="B281" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C281" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D281" s="4"/>
     </row>
@@ -5378,10 +5443,10 @@
         <v>261</v>
       </c>
       <c r="B282" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C282" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D282" s="4"/>
     </row>
@@ -5390,10 +5455,10 @@
         <v>262</v>
       </c>
       <c r="B283" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C283" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D283" s="4"/>
     </row>
@@ -5402,10 +5467,10 @@
         <v>263</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C284" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D284" s="4"/>
     </row>
@@ -5414,10 +5479,10 @@
         <v>264</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C285" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D285" s="4"/>
     </row>
@@ -5426,10 +5491,10 @@
         <v>265</v>
       </c>
       <c r="B286" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C286" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D286" s="4"/>
     </row>
@@ -5438,10 +5503,10 @@
         <v>266</v>
       </c>
       <c r="B287" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C287" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D287" s="4"/>
     </row>
@@ -5450,10 +5515,10 @@
         <v>267</v>
       </c>
       <c r="B288" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C288" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D288" s="4"/>
     </row>
@@ -5462,10 +5527,10 @@
         <v>268</v>
       </c>
       <c r="B289" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C289" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D289" s="4"/>
     </row>
@@ -5474,10 +5539,10 @@
         <v>269</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C290" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D290" s="4"/>
     </row>
@@ -5486,10 +5551,10 @@
         <v>270</v>
       </c>
       <c r="B291" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C291" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D291" s="4"/>
     </row>
@@ -5498,10 +5563,10 @@
         <v>271</v>
       </c>
       <c r="B292" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C292" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D292" s="4"/>
     </row>
@@ -5510,10 +5575,10 @@
         <v>272</v>
       </c>
       <c r="B293" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C293" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D293" s="4"/>
     </row>
@@ -5530,10 +5595,10 @@
         <v>273</v>
       </c>
       <c r="B296" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C296" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D296" s="4"/>
     </row>
@@ -5542,10 +5607,10 @@
         <v>274</v>
       </c>
       <c r="B297" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C297" s="6" t="s">
         <v>279</v>
-      </c>
-      <c r="C297" s="6" t="s">
-        <v>281</v>
       </c>
       <c r="D297" s="4"/>
     </row>
@@ -5554,10 +5619,10 @@
         <v>275</v>
       </c>
       <c r="B298" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C298" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D298" s="4"/>
     </row>
@@ -5566,10 +5631,10 @@
         <v>276</v>
       </c>
       <c r="B299" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C299" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D299" s="4"/>
     </row>
@@ -5578,10 +5643,10 @@
         <v>277</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D300" s="4"/>
     </row>
@@ -5590,10 +5655,10 @@
         <v>278</v>
       </c>
       <c r="B301" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C301" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D301" s="4"/>
     </row>
@@ -5602,10 +5667,10 @@
         <v>279</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C302" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D302" s="4"/>
     </row>
@@ -5614,10 +5679,10 @@
         <v>280</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C303" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D303" s="4"/>
     </row>
@@ -5626,10 +5691,10 @@
         <v>281</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C304" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D304" s="4"/>
     </row>
@@ -5638,10 +5703,10 @@
         <v>282</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C305" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D305" s="4"/>
     </row>
@@ -5650,10 +5715,10 @@
         <v>283</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C306" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D306" s="4"/>
     </row>
@@ -5662,10 +5727,10 @@
         <v>284</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C307" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D307" s="4"/>
     </row>
@@ -5674,10 +5739,10 @@
         <v>285</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C308" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D308" s="4"/>
     </row>
@@ -5686,10 +5751,10 @@
         <v>286</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D309" s="4"/>
     </row>
@@ -5698,10 +5763,10 @@
         <v>287</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C310" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D310" s="4"/>
     </row>
@@ -5710,10 +5775,10 @@
         <v>288</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C311" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D311" s="4"/>
     </row>
@@ -5722,10 +5787,10 @@
         <v>289</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C312" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D312" s="4"/>
     </row>
@@ -5734,10 +5799,10 @@
         <v>290</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C313" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D313" s="4"/>
     </row>
@@ -5746,10 +5811,10 @@
         <v>291</v>
       </c>
       <c r="B314" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C314" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D314" s="4"/>
     </row>
@@ -5758,10 +5823,10 @@
         <v>292</v>
       </c>
       <c r="B315" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C315" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D315" s="4"/>
     </row>
@@ -5770,10 +5835,10 @@
         <v>293</v>
       </c>
       <c r="B316" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C316" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D316" s="4"/>
     </row>
@@ -5782,10 +5847,10 @@
         <v>294</v>
       </c>
       <c r="B317" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C317" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D317" s="4"/>
     </row>
@@ -5794,10 +5859,10 @@
         <v>295</v>
       </c>
       <c r="B318" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C318" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D318" s="4"/>
     </row>
@@ -5806,10 +5871,10 @@
         <v>296</v>
       </c>
       <c r="B319" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C319" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D319" s="4"/>
     </row>
@@ -5818,10 +5883,10 @@
         <v>297</v>
       </c>
       <c r="B320" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C320" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D320" s="4"/>
     </row>
@@ -5830,10 +5895,10 @@
         <v>298</v>
       </c>
       <c r="B321" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C321" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D321" s="4"/>
     </row>
@@ -5842,10 +5907,10 @@
         <v>299</v>
       </c>
       <c r="B322" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C322" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D322" s="4"/>
     </row>
@@ -5854,10 +5919,10 @@
         <v>300</v>
       </c>
       <c r="B323" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C323" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D323" s="4"/>
     </row>
@@ -5866,10 +5931,10 @@
         <v>301</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C324" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D324" s="4"/>
     </row>
@@ -5878,10 +5943,10 @@
         <v>302</v>
       </c>
       <c r="B325" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C325" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D325" s="4"/>
     </row>
@@ -5890,10 +5955,10 @@
         <v>303</v>
       </c>
       <c r="B326" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C326" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D326" s="4"/>
     </row>
@@ -5902,10 +5967,10 @@
         <v>304</v>
       </c>
       <c r="B327" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C327" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D327" s="4"/>
     </row>
@@ -5914,10 +5979,10 @@
         <v>305</v>
       </c>
       <c r="B328" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C328" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D328" s="4"/>
     </row>
@@ -5926,10 +5991,10 @@
         <v>306</v>
       </c>
       <c r="B329" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C329" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D329" s="4"/>
     </row>
@@ -5938,10 +6003,10 @@
         <v>307</v>
       </c>
       <c r="B330" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C330" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D330" s="4"/>
     </row>
@@ -5950,10 +6015,10 @@
         <v>308</v>
       </c>
       <c r="B331" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C331" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D331" s="4"/>
     </row>
@@ -5962,10 +6027,10 @@
         <v>309</v>
       </c>
       <c r="B332" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C332" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D332" s="4"/>
     </row>
@@ -5974,10 +6039,10 @@
         <v>310</v>
       </c>
       <c r="B333" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C333" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D333" s="4"/>
     </row>
@@ -5991,163 +6056,163 @@
     </row>
     <row r="336" spans="1:4" ht="21">
       <c r="B336" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C336" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D336" s="4"/>
     </row>
     <row r="337" spans="2:4" ht="21">
       <c r="B337" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C337" s="6" t="s">
         <v>318</v>
-      </c>
-      <c r="C337" s="6" t="s">
-        <v>320</v>
       </c>
       <c r="D337" s="4"/>
     </row>
     <row r="338" spans="2:4" ht="21">
       <c r="B338" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C338" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D338" s="4"/>
     </row>
     <row r="339" spans="2:4" ht="21">
       <c r="B339" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D339" s="4"/>
     </row>
     <row r="340" spans="2:4" ht="21">
       <c r="B340" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C340" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D340" s="4"/>
     </row>
     <row r="341" spans="2:4" ht="21">
       <c r="B341" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C341" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D341" s="4"/>
     </row>
     <row r="342" spans="2:4" ht="21">
       <c r="B342" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C342" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D342" s="4"/>
     </row>
     <row r="343" spans="2:4" ht="21">
       <c r="B343" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C343" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D343" s="4"/>
     </row>
     <row r="344" spans="2:4" ht="21">
       <c r="B344" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D344" s="4"/>
     </row>
     <row r="345" spans="2:4" ht="21">
       <c r="B345" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C345" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D345" s="4"/>
     </row>
     <row r="346" spans="2:4" ht="21">
       <c r="B346" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C346" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D346" s="4"/>
     </row>
     <row r="347" spans="2:4" ht="21">
       <c r="B347" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C347" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D347" s="4"/>
     </row>
     <row r="348" spans="2:4" ht="21">
       <c r="B348" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C348" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D348" s="4"/>
     </row>
     <row r="349" spans="2:4" ht="21">
       <c r="B349" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C349" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D349" s="4"/>
     </row>
     <row r="350" spans="2:4" ht="21">
       <c r="B350" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C350" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D350" s="4"/>
     </row>
     <row r="351" spans="2:4" ht="21">
       <c r="B351" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C351" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D351" s="4"/>
     </row>
     <row r="352" spans="2:4" ht="21">
       <c r="B352" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C352" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D352" s="4"/>
     </row>
     <row r="353" spans="2:4" ht="21">
       <c r="B353" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C353" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D353" s="4"/>
     </row>
@@ -6161,397 +6226,397 @@
     </row>
     <row r="356" spans="2:4" ht="21">
       <c r="B356" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C356" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D356" s="4"/>
     </row>
     <row r="357" spans="2:4" ht="21">
       <c r="B357" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="C357" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="C357" s="6" t="s">
-        <v>339</v>
       </c>
       <c r="D357" s="4"/>
     </row>
     <row r="358" spans="2:4" ht="21">
       <c r="B358" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C358" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D358" s="4"/>
     </row>
     <row r="359" spans="2:4" ht="21">
       <c r="B359" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C359" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D359" s="4"/>
     </row>
     <row r="360" spans="2:4" ht="21">
       <c r="B360" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C360" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D360" s="4"/>
     </row>
     <row r="361" spans="2:4" ht="21">
       <c r="B361" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C361" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D361" s="4"/>
     </row>
     <row r="362" spans="2:4" ht="21">
       <c r="B362" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C362" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D362" s="4"/>
     </row>
     <row r="363" spans="2:4" ht="21">
       <c r="B363" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C363" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D363" s="4"/>
     </row>
     <row r="364" spans="2:4" ht="21">
       <c r="B364" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C364" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D364" s="4"/>
     </row>
     <row r="365" spans="2:4" ht="21">
       <c r="B365" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C365" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D365" s="4"/>
     </row>
     <row r="366" spans="2:4" ht="21">
       <c r="B366" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C366" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D366" s="4"/>
     </row>
     <row r="367" spans="2:4" ht="21">
       <c r="B367" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C367" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D367" s="4"/>
     </row>
     <row r="368" spans="2:4" ht="21">
       <c r="B368" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C368" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D368" s="4"/>
     </row>
     <row r="369" spans="2:4" ht="21">
       <c r="B369" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C369" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D369" s="4"/>
     </row>
     <row r="370" spans="2:4" ht="21">
       <c r="B370" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C370" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D370" s="4"/>
     </row>
     <row r="371" spans="2:4" ht="21">
       <c r="B371" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C371" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D371" s="4"/>
     </row>
     <row r="372" spans="2:4" ht="21">
       <c r="B372" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C372" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D372" s="4"/>
     </row>
     <row r="373" spans="2:4" ht="21">
       <c r="B373" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C373" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D373" s="4"/>
     </row>
     <row r="374" spans="2:4" ht="21">
       <c r="B374" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C374" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D374" s="4"/>
     </row>
     <row r="375" spans="2:4" ht="21">
       <c r="B375" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C375" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D375" s="4"/>
     </row>
     <row r="376" spans="2:4" ht="21">
       <c r="B376" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C376" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D376" s="4"/>
     </row>
     <row r="377" spans="2:4" ht="21">
       <c r="B377" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C377" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D377" s="4"/>
     </row>
     <row r="378" spans="2:4" ht="21">
       <c r="B378" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C378" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D378" s="4"/>
     </row>
     <row r="379" spans="2:4" ht="21">
       <c r="B379" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C379" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D379" s="4"/>
     </row>
     <row r="380" spans="2:4" ht="21">
       <c r="B380" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C380" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D380" s="4"/>
     </row>
     <row r="381" spans="2:4" ht="21">
       <c r="B381" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C381" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D381" s="4"/>
     </row>
     <row r="382" spans="2:4" ht="21">
       <c r="B382" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C382" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D382" s="4"/>
     </row>
     <row r="383" spans="2:4" ht="21">
       <c r="B383" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C383" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D383" s="4"/>
     </row>
     <row r="384" spans="2:4" ht="21">
       <c r="B384" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C384" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D384" s="4"/>
     </row>
     <row r="385" spans="2:4" ht="21">
       <c r="B385" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C385" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D385" s="4"/>
     </row>
     <row r="386" spans="2:4" ht="21">
       <c r="B386" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C386" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D386" s="4"/>
     </row>
     <row r="387" spans="2:4" ht="21">
       <c r="B387" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C387" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D387" s="4"/>
     </row>
     <row r="388" spans="2:4" ht="21">
       <c r="B388" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C388" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D388" s="4"/>
     </row>
     <row r="389" spans="2:4" ht="21">
       <c r="B389" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C389" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D389" s="4"/>
     </row>
     <row r="390" spans="2:4" ht="21">
       <c r="B390" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C390" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D390" s="4"/>
     </row>
     <row r="391" spans="2:4" ht="21">
       <c r="B391" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C391" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D391" s="4"/>
     </row>
     <row r="392" spans="2:4" ht="21">
       <c r="B392" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C392" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D392" s="4"/>
     </row>
     <row r="393" spans="2:4" ht="21">
       <c r="B393" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C393" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D393" s="4"/>
     </row>
     <row r="394" spans="2:4" ht="21">
       <c r="B394" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C394" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D394" s="4"/>
     </row>
     <row r="395" spans="2:4" ht="21">
       <c r="B395" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C395" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D395" s="4"/>
     </row>
     <row r="396" spans="2:4" ht="21">
       <c r="B396" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C396" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D396" s="4"/>
     </row>
     <row r="397" spans="2:4" ht="21">
       <c r="B397" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C397" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D397" s="4"/>
     </row>
     <row r="398" spans="2:4" ht="21">
       <c r="B398" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C398" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D398" s="4"/>
     </row>
     <row r="399" spans="2:4" ht="21">
       <c r="B399" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C399" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D399" s="4"/>
     </row>
@@ -6565,34 +6630,34 @@
     </row>
     <row r="402" spans="2:4" ht="21">
       <c r="B402" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C402" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D402" s="4"/>
     </row>
     <row r="403" spans="2:4" ht="21">
       <c r="B403" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C403" s="6" t="s">
         <v>381</v>
-      </c>
-      <c r="C403" s="6" t="s">
-        <v>383</v>
       </c>
       <c r="D403" s="4"/>
     </row>
     <row r="404" spans="2:4" ht="21">
       <c r="B404" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C404" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D404" s="4"/>
     </row>
     <row r="405" spans="2:4" ht="21">
       <c r="B405" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C405" s="6" t="s">
         <v>88</v>
@@ -6601,19 +6666,19 @@
     </row>
     <row r="406" spans="2:4" ht="21">
       <c r="B406" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C406" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D406" s="4"/>
     </row>
     <row r="407" spans="2:4" ht="21">
       <c r="B407" s="8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C407" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D407" s="4"/>
     </row>
@@ -6627,541 +6692,541 @@
     </row>
     <row r="410" spans="2:4" ht="21">
       <c r="B410" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C410" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D410" s="4"/>
     </row>
     <row r="411" spans="2:4" ht="21">
       <c r="B411" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C411" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="C411" s="6" t="s">
-        <v>389</v>
       </c>
       <c r="D411" s="4"/>
     </row>
     <row r="412" spans="2:4" ht="21">
       <c r="B412" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C412" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D412" s="4"/>
     </row>
     <row r="413" spans="2:4" ht="21">
       <c r="B413" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C413" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D413" s="4"/>
     </row>
     <row r="414" spans="2:4" ht="21">
       <c r="B414" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C414" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D414" s="4"/>
     </row>
     <row r="415" spans="2:4" ht="21">
       <c r="B415" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C415" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D415" s="4"/>
     </row>
     <row r="416" spans="2:4" ht="21">
       <c r="B416" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C416" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D416" s="4"/>
     </row>
     <row r="417" spans="2:4" ht="21">
       <c r="B417" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C417" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D417" s="4"/>
     </row>
     <row r="418" spans="2:4" ht="21">
       <c r="B418" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C418" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D418" s="4"/>
     </row>
     <row r="419" spans="2:4" ht="21">
       <c r="B419" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C419" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D419" s="4"/>
     </row>
     <row r="420" spans="2:4" ht="21">
       <c r="B420" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C420" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D420" s="4"/>
     </row>
     <row r="421" spans="2:4" ht="21">
       <c r="B421" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C421" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D421" s="4"/>
     </row>
     <row r="422" spans="2:4" ht="21">
       <c r="B422" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C422" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D422" s="4"/>
     </row>
     <row r="423" spans="2:4" ht="21">
       <c r="B423" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C423" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D423" s="4"/>
     </row>
     <row r="424" spans="2:4" ht="21">
       <c r="B424" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C424" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D424" s="4"/>
     </row>
     <row r="425" spans="2:4" ht="21">
       <c r="B425" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C425" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D425" s="4"/>
     </row>
     <row r="426" spans="2:4" ht="21">
       <c r="B426" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C426" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D426" s="4"/>
     </row>
     <row r="427" spans="2:4" ht="21">
       <c r="B427" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C427" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D427" s="4"/>
     </row>
     <row r="428" spans="2:4" ht="21">
       <c r="B428" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C428" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D428" s="4"/>
     </row>
     <row r="429" spans="2:4" ht="21">
       <c r="B429" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C429" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D429" s="4"/>
     </row>
     <row r="430" spans="2:4" ht="21">
       <c r="B430" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C430" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D430" s="4"/>
     </row>
     <row r="431" spans="2:4" ht="21">
       <c r="B431" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C431" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D431" s="4"/>
     </row>
     <row r="432" spans="2:4" ht="21">
       <c r="B432" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C432" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D432" s="4"/>
     </row>
     <row r="433" spans="2:4" ht="21">
       <c r="B433" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C433" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D433" s="4"/>
     </row>
     <row r="434" spans="2:4" ht="21">
       <c r="B434" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C434" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D434" s="4"/>
     </row>
     <row r="435" spans="2:4" ht="21">
       <c r="B435" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C435" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D435" s="4"/>
     </row>
     <row r="436" spans="2:4" ht="21">
       <c r="B436" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C436" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D436" s="4"/>
     </row>
     <row r="437" spans="2:4" ht="21">
       <c r="B437" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C437" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D437" s="4"/>
     </row>
     <row r="438" spans="2:4" ht="21">
       <c r="B438" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C438" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D438" s="4"/>
     </row>
     <row r="439" spans="2:4" ht="21">
       <c r="B439" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C439" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D439" s="4"/>
     </row>
     <row r="440" spans="2:4" ht="21">
       <c r="B440" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C440" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D440" s="4"/>
     </row>
     <row r="441" spans="2:4" ht="21">
       <c r="B441" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C441" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D441" s="4"/>
     </row>
     <row r="442" spans="2:4" ht="21">
       <c r="B442" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C442" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D442" s="4"/>
     </row>
     <row r="443" spans="2:4" ht="21">
       <c r="B443" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C443" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D443" s="4"/>
     </row>
     <row r="444" spans="2:4" ht="21">
       <c r="B444" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C444" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D444" s="4"/>
     </row>
     <row r="445" spans="2:4" ht="21">
       <c r="B445" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C445" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D445" s="4"/>
     </row>
     <row r="446" spans="2:4" ht="21">
       <c r="B446" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C446" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D446" s="4"/>
     </row>
     <row r="447" spans="2:4" ht="21">
       <c r="B447" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C447" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D447" s="4"/>
     </row>
     <row r="448" spans="2:4" ht="21">
       <c r="B448" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C448" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D448" s="4"/>
     </row>
     <row r="449" spans="2:4" ht="21">
       <c r="B449" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C449" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D449" s="4"/>
     </row>
     <row r="450" spans="2:4" ht="21">
       <c r="B450" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C450" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D450" s="4"/>
     </row>
     <row r="451" spans="2:4" ht="21">
       <c r="B451" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C451" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D451" s="4"/>
     </row>
     <row r="452" spans="2:4" ht="21">
       <c r="B452" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C452" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D452" s="4"/>
     </row>
     <row r="453" spans="2:4" ht="21">
       <c r="B453" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C453" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D453" s="4"/>
     </row>
     <row r="454" spans="2:4" ht="21">
       <c r="B454" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C454" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D454" s="4"/>
     </row>
     <row r="455" spans="2:4" ht="21">
       <c r="B455" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C455" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D455" s="4"/>
     </row>
     <row r="456" spans="2:4" ht="21">
       <c r="B456" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C456" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D456" s="4"/>
     </row>
     <row r="457" spans="2:4" ht="21">
       <c r="B457" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C457" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D457" s="4"/>
     </row>
     <row r="458" spans="2:4" ht="21">
       <c r="B458" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C458" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D458" s="4"/>
     </row>
     <row r="459" spans="2:4" ht="21">
       <c r="B459" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C459" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D459" s="4"/>
     </row>
     <row r="460" spans="2:4" ht="21">
       <c r="B460" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C460" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D460" s="4"/>
     </row>
     <row r="461" spans="2:4" ht="21">
       <c r="B461" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C461" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D461" s="4"/>
     </row>
     <row r="462" spans="2:4" ht="21">
       <c r="B462" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C462" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D462" s="4"/>
     </row>
     <row r="463" spans="2:4" ht="21">
       <c r="B463" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C463" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D463" s="4"/>
     </row>
     <row r="464" spans="2:4" ht="21">
       <c r="B464" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C464" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D464" s="4"/>
     </row>
     <row r="465" spans="2:4" ht="21">
       <c r="B465" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C465" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D465" s="4"/>
     </row>
     <row r="466" spans="2:4" ht="21">
       <c r="B466" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C466" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D466" s="4"/>
     </row>
     <row r="467" spans="2:4" ht="21">
       <c r="B467" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C467" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D467" s="4"/>
     </row>
     <row r="468" spans="2:4" ht="21">
       <c r="B468" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C468" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D468" s="4"/>
     </row>
     <row r="469" spans="2:4" ht="21">
       <c r="B469" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C469" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D469" s="4"/>
     </row>
@@ -7176,98 +7241,98 @@
     </row>
     <row r="472" spans="2:4" ht="21">
       <c r="B472" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C472" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D472" s="4"/>
     </row>
     <row r="473" spans="2:4" ht="21">
       <c r="B473" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="C473" s="6" t="s">
         <v>447</v>
-      </c>
-      <c r="C473" s="6" t="s">
-        <v>449</v>
       </c>
       <c r="D473" s="4"/>
     </row>
     <row r="474" spans="2:4" ht="21">
       <c r="B474" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C474" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D474" s="4"/>
     </row>
     <row r="475" spans="2:4" ht="21">
       <c r="B475" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C475" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D475" s="4"/>
     </row>
     <row r="476" spans="2:4" ht="21">
       <c r="B476" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C476" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D476" s="4"/>
     </row>
     <row r="477" spans="2:4" ht="21">
       <c r="B477" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C477" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D477" s="4"/>
     </row>
     <row r="478" spans="2:4" ht="21">
       <c r="B478" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C478" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D478" s="4"/>
     </row>
     <row r="479" spans="2:4" ht="21">
       <c r="B479" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C479" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D479" s="4"/>
     </row>
     <row r="480" spans="2:4" ht="21">
       <c r="B480" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C480" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D480" s="4"/>
     </row>
     <row r="481" spans="2:4" ht="21">
       <c r="B481" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C481" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D481" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D481" xr:uid="{BB54F377-8C14-4DE8-8D78-249FF92CBC7B}">
-      <formula1>$H$2:$H$3</formula1>
+      <formula1>$I$2:$I$3</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -7422,8 +7487,8 @@
     <hyperlink ref="C163" r:id="rId149" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
     <hyperlink ref="C166" r:id="rId150" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
     <hyperlink ref="C167" r:id="rId151" display="Sort a LL of 0's, 1's and 2's" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
-    <hyperlink ref="C168" r:id="rId152" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
-    <hyperlink ref="C169" r:id="rId153" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
+    <hyperlink ref="C168" r:id="rId152" display="Clone a linked list with next and random pointer" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
+    <hyperlink ref="C169" r:id="rId153" display="Merge K sorted Linked list" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
     <hyperlink ref="C170" r:id="rId154" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
     <hyperlink ref="C171" r:id="rId155" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
     <hyperlink ref="C172" r:id="rId156" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>

</xml_diff>

<commit_message>
Day 10 (Backtracking complete)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psharm03\Documents\GitHub\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784148CC-684E-48E7-90AC-D24001915976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE4DB65-F930-46B9-8894-3ACD08AAC9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Table1!$A$1:$A$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="479">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1468,7 +1467,19 @@
     <t>O(nm)</t>
   </si>
   <si>
-    <t>Print all Subsequences of a string. [Include/Exclude Method]</t>
+    <t>Print all Subsequences of a string. [Include/Exclude Method] [Solve by bitwise]</t>
+  </si>
+  <si>
+    <t>O()</t>
+  </si>
+  <si>
+    <t>O(4^n^2)</t>
+  </si>
+  <si>
+    <t>O(n!)</t>
+  </si>
+  <si>
+    <t>O(n*n)</t>
   </si>
 </sst>
 </file>
@@ -2014,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:I481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A264" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2778,16 +2789,22 @@
       <c r="F65" s="21"/>
     </row>
     <row r="66" spans="1:6" ht="21">
-      <c r="A66">
+      <c r="A66" s="12">
         <v>57</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D66" s="4"/>
+      <c r="D66" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="F66" s="12"/>
     </row>
     <row r="67" spans="1:6" ht="21">
       <c r="A67">
@@ -5381,39 +5398,53 @@
       </c>
       <c r="D272" s="4"/>
     </row>
-    <row r="273" spans="1:4" ht="21">
+    <row r="273" spans="1:6" ht="21">
       <c r="C273" s="7"/>
       <c r="D273" s="4"/>
     </row>
-    <row r="274" spans="1:4" ht="21">
+    <row r="274" spans="1:6" ht="21">
       <c r="C274" s="7"/>
       <c r="D274" s="4"/>
     </row>
-    <row r="275" spans="1:4" ht="21">
-      <c r="A275">
+    <row r="275" spans="1:6" ht="21">
+      <c r="A275" s="12">
         <v>254</v>
       </c>
-      <c r="B275" s="5" t="s">
+      <c r="B275" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C275" s="6" t="s">
+      <c r="C275" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="D275" s="4"/>
-    </row>
-    <row r="276" spans="1:4" ht="21">
-      <c r="A276">
+      <c r="D275" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="E275" s="12" t="s">
+        <v>476</v>
+      </c>
+      <c r="F275" s="12"/>
+    </row>
+    <row r="276" spans="1:6" ht="21">
+      <c r="A276" s="12">
         <v>255</v>
       </c>
-      <c r="B276" s="5" t="s">
+      <c r="B276" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C276" s="6" t="s">
+      <c r="C276" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="D276" s="4"/>
-    </row>
-    <row r="277" spans="1:4" ht="21">
+      <c r="D276" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="E276" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="F276" s="12" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="21">
       <c r="A277">
         <v>256</v>
       </c>
@@ -5425,7 +5456,7 @@
       </c>
       <c r="D277" s="4"/>
     </row>
-    <row r="278" spans="1:4" ht="21">
+    <row r="278" spans="1:6" ht="21">
       <c r="A278">
         <v>257</v>
       </c>
@@ -5437,19 +5468,21 @@
       </c>
       <c r="D278" s="4"/>
     </row>
-    <row r="279" spans="1:4" ht="21">
-      <c r="A279">
+    <row r="279" spans="1:6" ht="21">
+      <c r="A279" s="12">
         <v>258</v>
       </c>
-      <c r="B279" s="5" t="s">
+      <c r="B279" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C279" s="6" t="s">
+      <c r="C279" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="D279" s="4"/>
-    </row>
-    <row r="280" spans="1:4" ht="21">
+      <c r="D279" s="15"/>
+      <c r="E279" s="12"/>
+      <c r="F279" s="12"/>
+    </row>
+    <row r="280" spans="1:6" ht="21">
       <c r="A280">
         <v>259</v>
       </c>
@@ -5461,7 +5494,7 @@
       </c>
       <c r="D280" s="4"/>
     </row>
-    <row r="281" spans="1:4" ht="21">
+    <row r="281" spans="1:6" ht="21">
       <c r="A281">
         <v>260</v>
       </c>
@@ -5473,7 +5506,7 @@
       </c>
       <c r="D281" s="4"/>
     </row>
-    <row r="282" spans="1:4" ht="21">
+    <row r="282" spans="1:6" ht="21">
       <c r="A282">
         <v>261</v>
       </c>
@@ -5485,7 +5518,7 @@
       </c>
       <c r="D282" s="4"/>
     </row>
-    <row r="283" spans="1:4" ht="21">
+    <row r="283" spans="1:6" ht="21">
       <c r="A283">
         <v>262</v>
       </c>
@@ -5497,7 +5530,7 @@
       </c>
       <c r="D283" s="4"/>
     </row>
-    <row r="284" spans="1:4" ht="21">
+    <row r="284" spans="1:6" ht="21">
       <c r="A284">
         <v>263</v>
       </c>
@@ -5509,7 +5542,7 @@
       </c>
       <c r="D284" s="4"/>
     </row>
-    <row r="285" spans="1:4" ht="21">
+    <row r="285" spans="1:6" ht="21">
       <c r="A285">
         <v>264</v>
       </c>
@@ -5521,7 +5554,7 @@
       </c>
       <c r="D285" s="4"/>
     </row>
-    <row r="286" spans="1:4" ht="21">
+    <row r="286" spans="1:6" ht="21">
       <c r="A286">
         <v>265</v>
       </c>
@@ -5533,7 +5566,7 @@
       </c>
       <c r="D286" s="4"/>
     </row>
-    <row r="287" spans="1:4" ht="21">
+    <row r="287" spans="1:6" ht="21">
       <c r="A287">
         <v>266</v>
       </c>
@@ -5545,7 +5578,7 @@
       </c>
       <c r="D287" s="4"/>
     </row>
-    <row r="288" spans="1:4" ht="21">
+    <row r="288" spans="1:6" ht="21">
       <c r="A288">
         <v>267</v>
       </c>

</xml_diff>